<commit_message>
NAGA optimization based on PSA simulation
</commit_message>
<xml_diff>
--- a/simulation/multicomponentPSA/graph/LangmuirParameters.xlsx
+++ b/simulation/multicomponentPSA/graph/LangmuirParameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Simulation\ProjectApolloSimulation\simulation\multicomponentPSA\graph\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FECE33BA-2E43-4BC7-A97E-F31FD2D49D9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A20CE2-8662-444A-BBD3-FD2270734961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2325" yWindow="2055" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -669,10 +669,13 @@
   <dimension ref="A1:AE9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:I9"/>
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="11" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.15">
       <c r="B1" s="1" t="s">

</xml_diff>